<commit_message>
modified:   Deepin/Installation_Guide.md 	modified:   Deepin/deepin_setup.sh 	deleted:    "Test/Firefox/\346\265\213\350\257\225\347\224\250\344\276\213\344\270\216\347\274\272\351\231\267\346\212\245\345\221\212/.~\345\272\204\344\270\234\347\224\237 firefox\345\256\211\350\243\205\357\274\214\346\265\213\350\257\225\347\224\250\344\276\213\344\270\216\347\274\272\351\231\267_120024_1657082649880.xlsx" 	modified:   "Test/Firefox/\346\265\213\350\257\225\347\224\250\344\276\213\344\270\216\347\274\272\351\231\267\346\212\245\345\221\212/\345\272\204\344\270\234\347\224\237 firefox\345\256\211\350\243\205\357\274\214\346\265\213\350\257\225\347\224\250\344\276\213\344\270\216\347\274\272\351\231\267_120024_1657082649880.xlsx"
</commit_message>
<xml_diff>
--- a/Test/Firefox/测试用例与缺陷报告/庄东生 firefox安装，测试用例与缺陷_120024_1657082649880.xlsx
+++ b/Test/Firefox/测试用例与缺陷报告/庄东生 firefox安装，测试用例与缺陷_120024_1657082649880.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9420"/>
+    <workbookView windowWidth="11472" windowHeight="10656"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1278,16 +1278,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1295,57 +1295,51 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="24"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="22"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -1353,7 +1347,38 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -1361,14 +1386,45 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -1376,84 +1432,28 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -1479,55 +1479,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1545,67 +1509,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1623,7 +1551,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1635,7 +1587,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1647,19 +1641,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1688,6 +1688,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1699,54 +1708,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1769,8 +1730,38 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1785,157 +1776,166 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2014,15 +2014,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2031,55 +2025,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2120,8 +2114,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9532620" y="11457305"/>
-          <a:ext cx="1459230" cy="719455"/>
+          <a:off x="10564495" y="11533505"/>
+          <a:ext cx="1614170" cy="719455"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2162,8 +2156,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9555480" y="9845040"/>
-          <a:ext cx="1596390" cy="820420"/>
+          <a:off x="10587355" y="9822180"/>
+          <a:ext cx="1751330" cy="820420"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2204,8 +2198,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9425940" y="8272780"/>
-          <a:ext cx="1590040" cy="939800"/>
+          <a:off x="10457815" y="8249920"/>
+          <a:ext cx="1744980" cy="939800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2246,8 +2240,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9418320" y="12799060"/>
-          <a:ext cx="1398905" cy="784860"/>
+          <a:off x="10450195" y="12974320"/>
+          <a:ext cx="1553845" cy="784860"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2288,8 +2282,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9418320" y="14269085"/>
-          <a:ext cx="1492250" cy="824865"/>
+          <a:off x="10450195" y="14543405"/>
+          <a:ext cx="1647190" cy="824865"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2330,8 +2324,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9624060" y="15770860"/>
-          <a:ext cx="1482725" cy="831215"/>
+          <a:off x="10655935" y="16144240"/>
+          <a:ext cx="1637665" cy="831215"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2372,8 +2366,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9471660" y="18940780"/>
-          <a:ext cx="1939290" cy="868680"/>
+          <a:off x="10503535" y="19367500"/>
+          <a:ext cx="2162810" cy="868680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2414,8 +2408,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9570720" y="17203420"/>
-          <a:ext cx="1563370" cy="907415"/>
+          <a:off x="10602595" y="17675860"/>
+          <a:ext cx="1718310" cy="907415"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2456,8 +2450,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9768840" y="20480020"/>
-          <a:ext cx="1287145" cy="663575"/>
+          <a:off x="10800715" y="21005800"/>
+          <a:ext cx="1442085" cy="663575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2498,8 +2492,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9723120" y="22110700"/>
-          <a:ext cx="1527810" cy="572770"/>
+          <a:off x="10754995" y="22735540"/>
+          <a:ext cx="1682750" cy="572770"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2540,8 +2534,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9761220" y="23436580"/>
-          <a:ext cx="1325880" cy="732790"/>
+          <a:off x="10793095" y="24160480"/>
+          <a:ext cx="1480820" cy="732790"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2582,8 +2576,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9776460" y="24975820"/>
-          <a:ext cx="1153160" cy="609600"/>
+          <a:off x="10808335" y="25798780"/>
+          <a:ext cx="1308100" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2624,8 +2618,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="9942195" y="26286460"/>
-          <a:ext cx="1235710" cy="610235"/>
+          <a:off x="10974070" y="27208480"/>
+          <a:ext cx="1390650" cy="610235"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2666,8 +2660,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9670415" y="33870265"/>
-          <a:ext cx="1409065" cy="585470"/>
+          <a:off x="10702290" y="35287585"/>
+          <a:ext cx="1564005" cy="585470"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2708,8 +2702,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9852660" y="35369500"/>
-          <a:ext cx="1082040" cy="601980"/>
+          <a:off x="10884535" y="36885880"/>
+          <a:ext cx="1236980" cy="601980"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2750,8 +2744,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9814560" y="36794440"/>
-          <a:ext cx="1342390" cy="701675"/>
+          <a:off x="10846435" y="38409880"/>
+          <a:ext cx="1497330" cy="701675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2792,8 +2786,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9608820" y="27863800"/>
-          <a:ext cx="1476375" cy="723900"/>
+          <a:off x="10640695" y="28884880"/>
+          <a:ext cx="1631315" cy="723900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2834,8 +2828,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9822180" y="29433520"/>
-          <a:ext cx="1425575" cy="518795"/>
+          <a:off x="10854055" y="30553660"/>
+          <a:ext cx="1580515" cy="518795"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2876,8 +2870,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9822180" y="30843220"/>
-          <a:ext cx="1264920" cy="647700"/>
+          <a:off x="10854055" y="32062420"/>
+          <a:ext cx="1419860" cy="647700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2918,8 +2912,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9517380" y="32245300"/>
-          <a:ext cx="1615440" cy="739140"/>
+          <a:off x="10549255" y="33563560"/>
+          <a:ext cx="1770380" cy="739140"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2960,8 +2954,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9745980" y="38272720"/>
-          <a:ext cx="1181735" cy="539115"/>
+          <a:off x="10777855" y="39987220"/>
+          <a:ext cx="1336675" cy="539115"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3002,8 +2996,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9563100" y="42539920"/>
-          <a:ext cx="1623060" cy="944880"/>
+          <a:off x="10594975" y="44368720"/>
+          <a:ext cx="1778000" cy="944880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3044,8 +3038,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9638665" y="44140120"/>
-          <a:ext cx="1311910" cy="739775"/>
+          <a:off x="10670540" y="46067980"/>
+          <a:ext cx="1466850" cy="739775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3086,8 +3080,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9822180" y="45641260"/>
-          <a:ext cx="1067435" cy="511175"/>
+          <a:off x="10854055" y="47668180"/>
+          <a:ext cx="1222375" cy="511175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3128,7 +3122,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9738360" y="47073820"/>
+          <a:off x="10770235" y="49199800"/>
           <a:ext cx="884555" cy="556260"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3170,8 +3164,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9791700" y="48741965"/>
-          <a:ext cx="1082675" cy="466090"/>
+          <a:off x="10823575" y="50967005"/>
+          <a:ext cx="1237615" cy="466090"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3212,8 +3206,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9753600" y="39842440"/>
-          <a:ext cx="1409700" cy="617220"/>
+          <a:off x="10785475" y="41473120"/>
+          <a:ext cx="1564640" cy="617220"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3254,8 +3248,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9745980" y="41381680"/>
-          <a:ext cx="1174115" cy="777875"/>
+          <a:off x="10777855" y="43111420"/>
+          <a:ext cx="1329055" cy="777875"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3296,8 +3290,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9662160" y="51530885"/>
-          <a:ext cx="1584325" cy="732790"/>
+          <a:off x="10694035" y="53954045"/>
+          <a:ext cx="1739265" cy="732790"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3338,8 +3332,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9966960" y="52941220"/>
-          <a:ext cx="1121410" cy="581025"/>
+          <a:off x="10998835" y="55463440"/>
+          <a:ext cx="1276350" cy="581025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3380,8 +3374,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9776460" y="55844440"/>
-          <a:ext cx="1226820" cy="510540"/>
+          <a:off x="10808335" y="58564780"/>
+          <a:ext cx="1381760" cy="510540"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3422,8 +3416,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9989820" y="58694320"/>
-          <a:ext cx="1135380" cy="716280"/>
+          <a:off x="11021695" y="61612780"/>
+          <a:ext cx="1290320" cy="716280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3464,8 +3458,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9715500" y="60264040"/>
-          <a:ext cx="1348105" cy="557530"/>
+          <a:off x="10747375" y="63281560"/>
+          <a:ext cx="1503045" cy="557530"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3506,8 +3500,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9890760" y="57406540"/>
-          <a:ext cx="1379220" cy="525780"/>
+          <a:off x="10922635" y="60225940"/>
+          <a:ext cx="1534160" cy="525780"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3548,8 +3542,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9471660" y="63334900"/>
-          <a:ext cx="1381760" cy="556260"/>
+          <a:off x="10503535" y="66565780"/>
+          <a:ext cx="1536700" cy="556260"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3590,8 +3584,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9441180" y="66375280"/>
-          <a:ext cx="1447165" cy="557530"/>
+          <a:off x="10473055" y="69804280"/>
+          <a:ext cx="1602105" cy="557530"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3632,7 +3626,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9601200" y="69232780"/>
+          <a:off x="10633075" y="72859900"/>
           <a:ext cx="925195" cy="548640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3674,7 +3668,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9364980" y="70733920"/>
+          <a:off x="10396855" y="74460100"/>
           <a:ext cx="1155065" cy="511175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3716,7 +3710,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="9486900" y="67869435"/>
+          <a:off x="10518775" y="71397495"/>
           <a:ext cx="1033145" cy="524510"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3758,7 +3752,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9474835" y="73553320"/>
+          <a:off x="10506710" y="77477620"/>
           <a:ext cx="1056005" cy="510540"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3800,7 +3794,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9494520" y="75161140"/>
+          <a:off x="10526395" y="79184500"/>
           <a:ext cx="1050290" cy="541655"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3842,8 +3836,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9540240" y="76525120"/>
-          <a:ext cx="1328420" cy="685800"/>
+          <a:off x="10572115" y="80647540"/>
+          <a:ext cx="1483360" cy="685800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3884,7 +3878,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9441180" y="79550260"/>
+          <a:off x="10473055" y="83870800"/>
           <a:ext cx="1181735" cy="514350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3926,8 +3920,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9685020" y="78056740"/>
-          <a:ext cx="1014730" cy="563880"/>
+          <a:off x="10716895" y="82278220"/>
+          <a:ext cx="1169670" cy="563880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3968,7 +3962,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9494520" y="80891380"/>
+          <a:off x="10526395" y="85310980"/>
           <a:ext cx="1044575" cy="571500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4010,7 +4004,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9387840" y="82445860"/>
+          <a:off x="10419715" y="86964520"/>
           <a:ext cx="1181735" cy="440055"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4052,7 +4046,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9319260" y="72219820"/>
+          <a:off x="10351135" y="76045060"/>
           <a:ext cx="1166495" cy="473075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4094,7 +4088,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9540240" y="83893660"/>
+          <a:off x="10572115" y="88511380"/>
           <a:ext cx="998220" cy="606425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4136,7 +4130,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9654540" y="101473000"/>
+          <a:off x="10686415" y="107279440"/>
           <a:ext cx="799465" cy="403860"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4178,7 +4172,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9463405" y="100063935"/>
+          <a:off x="10495280" y="105771315"/>
           <a:ext cx="1172210" cy="682625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4220,7 +4214,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9410700" y="102760780"/>
+          <a:off x="10442575" y="108666280"/>
           <a:ext cx="1139190" cy="586740"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4262,8 +4256,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9418320" y="96984820"/>
-          <a:ext cx="1769745" cy="563880"/>
+          <a:off x="10450195" y="102494080"/>
+          <a:ext cx="1924685" cy="563880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4304,8 +4298,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9281160" y="98318320"/>
-          <a:ext cx="1550035" cy="655955"/>
+          <a:off x="10218420" y="103926640"/>
+          <a:ext cx="1799590" cy="655955"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4346,7 +4340,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9349740" y="85371940"/>
+          <a:off x="10381615" y="90088720"/>
           <a:ext cx="1296670" cy="632460"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4388,8 +4382,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="9410700" y="86680040"/>
-          <a:ext cx="1524000" cy="627380"/>
+          <a:off x="10442575" y="91495880"/>
+          <a:ext cx="1678940" cy="627380"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4430,7 +4424,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9456420" y="89783920"/>
+          <a:off x="10488295" y="94797880"/>
           <a:ext cx="744855" cy="427355"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4472,8 +4466,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9646920" y="91064080"/>
-          <a:ext cx="1270635" cy="784860"/>
+          <a:off x="10678795" y="96177100"/>
+          <a:ext cx="1425575" cy="784860"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4514,8 +4508,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9913620" y="95460820"/>
-          <a:ext cx="1029335" cy="552450"/>
+          <a:off x="10945495" y="100871020"/>
+          <a:ext cx="1184275" cy="552450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4556,8 +4550,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9578340" y="92671900"/>
-          <a:ext cx="1303655" cy="621030"/>
+          <a:off x="10610215" y="97883980"/>
+          <a:ext cx="1458595" cy="621030"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4598,8 +4592,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9852660" y="94279720"/>
-          <a:ext cx="1066800" cy="465455"/>
+          <a:off x="10884535" y="99590860"/>
+          <a:ext cx="1221740" cy="465455"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4640,8 +4634,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9555480" y="9591040"/>
-          <a:ext cx="1436370" cy="843915"/>
+          <a:off x="10587355" y="9568180"/>
+          <a:ext cx="1591310" cy="843915"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4682,8 +4676,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9616440" y="88290400"/>
-          <a:ext cx="1074420" cy="502920"/>
+          <a:off x="10648315" y="93205300"/>
+          <a:ext cx="1229360" cy="502920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4724,8 +4718,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8839200" y="1203960"/>
-          <a:ext cx="5273675" cy="930910"/>
+          <a:off x="9776460" y="1203960"/>
+          <a:ext cx="5866130" cy="930910"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4766,8 +4760,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9075420" y="2537460"/>
-          <a:ext cx="4389120" cy="1676400"/>
+          <a:off x="10012680" y="2537460"/>
+          <a:ext cx="4912995" cy="1676400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4808,8 +4802,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3940175" y="4419600"/>
-          <a:ext cx="3522345" cy="2278380"/>
+          <a:off x="4298315" y="4419600"/>
+          <a:ext cx="3956685" cy="2278380"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4832,8 +4826,8 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>592455</xdr:colOff>
-      <xdr:row>89</xdr:row>
-      <xdr:rowOff>3175</xdr:rowOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>734695</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4850,8 +4844,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10721340" y="105318560"/>
-          <a:ext cx="1171575" cy="574675"/>
+          <a:off x="11908155" y="111292640"/>
+          <a:ext cx="1240155" cy="574675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4892,8 +4886,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10942320" y="106301540"/>
-          <a:ext cx="1066800" cy="465455"/>
+          <a:off x="12129135" y="112313720"/>
+          <a:ext cx="1203960" cy="465455"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5198,14 +5192,14 @@
   <sheetPr/>
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="M94" sqref="M94"/>
+    <sheetView tabSelected="1" topLeftCell="B82" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
     <col min="2" max="7" width="19" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.4444444444444" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.4416666666667" style="3" customWidth="1"/>
     <col min="9" max="9" width="20.3333333333333" style="4" customWidth="1"/>
     <col min="10" max="10" width="9" style="4"/>
   </cols>
@@ -5471,7 +5465,7 @@
       <c r="J19" s="21"/>
       <c r="N19" s="13"/>
     </row>
-    <row r="20" ht="115.2" spans="1:10">
+    <row r="20" ht="123" spans="1:10">
       <c r="A20" s="10"/>
       <c r="B20" s="16" t="s">
         <v>23</v>
@@ -5497,7 +5491,7 @@
       <c r="I20" s="12"/>
       <c r="J20" s="18"/>
     </row>
-    <row r="21" ht="115.2" spans="1:10">
+    <row r="21" ht="123" spans="1:10">
       <c r="A21" s="10"/>
       <c r="B21" s="16" t="s">
         <v>29</v>
@@ -5523,7 +5517,7 @@
       <c r="I21" s="12"/>
       <c r="J21" s="18"/>
     </row>
-    <row r="22" ht="115.2" spans="1:10">
+    <row r="22" ht="123" spans="1:10">
       <c r="A22" s="10"/>
       <c r="B22" s="16" t="s">
         <v>33</v>
@@ -5549,7 +5543,7 @@
       <c r="I22" s="12"/>
       <c r="J22" s="18"/>
     </row>
-    <row r="23" ht="115.2" spans="1:10">
+    <row r="23" ht="123" spans="1:10">
       <c r="A23" s="10"/>
       <c r="B23" s="16" t="s">
         <v>37</v>
@@ -5575,7 +5569,7 @@
       <c r="I23" s="12"/>
       <c r="J23" s="18"/>
     </row>
-    <row r="24" ht="115.2" spans="1:10">
+    <row r="24" ht="123" spans="1:10">
       <c r="A24" s="10"/>
       <c r="B24" s="16" t="s">
         <v>41</v>
@@ -5601,7 +5595,7 @@
       <c r="I24" s="12"/>
       <c r="J24" s="18"/>
     </row>
-    <row r="25" ht="144" spans="1:10">
+    <row r="25" ht="140.4" spans="1:10">
       <c r="A25" s="10"/>
       <c r="B25" s="16" t="s">
         <v>45</v>
@@ -5627,7 +5621,7 @@
       <c r="I25" s="12"/>
       <c r="J25" s="18"/>
     </row>
-    <row r="26" ht="115.2" spans="1:10">
+    <row r="26" ht="123" spans="1:10">
       <c r="A26" s="10"/>
       <c r="B26" s="16" t="s">
         <v>50</v>
@@ -5653,7 +5647,7 @@
       <c r="I26" s="12"/>
       <c r="J26" s="18"/>
     </row>
-    <row r="27" ht="115.2" spans="1:10">
+    <row r="27" ht="123" spans="1:10">
       <c r="A27" s="10"/>
       <c r="B27" s="16" t="s">
         <v>55</v>
@@ -5679,7 +5673,7 @@
       <c r="I27" s="12"/>
       <c r="J27" s="18"/>
     </row>
-    <row r="28" ht="115.2" spans="1:10">
+    <row r="28" ht="123" spans="1:10">
       <c r="A28" s="10"/>
       <c r="B28" s="16" t="s">
         <v>59</v>
@@ -5705,7 +5699,7 @@
       <c r="I28" s="12"/>
       <c r="J28" s="18"/>
     </row>
-    <row r="29" ht="115.2" spans="1:10">
+    <row r="29" ht="123" spans="1:10">
       <c r="A29" s="10"/>
       <c r="B29" s="16" t="s">
         <v>64</v>
@@ -5731,7 +5725,7 @@
       <c r="I29" s="12"/>
       <c r="J29" s="18"/>
     </row>
-    <row r="30" ht="115.2" spans="1:10">
+    <row r="30" ht="123" spans="1:10">
       <c r="A30" s="10"/>
       <c r="B30" s="16" t="s">
         <v>66</v>
@@ -5757,7 +5751,7 @@
       <c r="I30" s="12"/>
       <c r="J30" s="18"/>
     </row>
-    <row r="31" ht="115.2" spans="1:10">
+    <row r="31" ht="123" spans="1:10">
       <c r="A31" s="10"/>
       <c r="B31" s="16" t="s">
         <v>71</v>
@@ -5783,7 +5777,7 @@
       <c r="I31" s="12"/>
       <c r="J31" s="18"/>
     </row>
-    <row r="32" ht="115.2" spans="1:10">
+    <row r="32" ht="123" spans="1:10">
       <c r="A32" s="10"/>
       <c r="B32" s="16" t="s">
         <v>76</v>
@@ -5809,7 +5803,7 @@
       <c r="I32" s="12"/>
       <c r="J32" s="18"/>
     </row>
-    <row r="33" ht="115.2" spans="1:10">
+    <row r="33" ht="123" spans="1:10">
       <c r="A33" s="10"/>
       <c r="B33" s="16" t="s">
         <v>80</v>
@@ -5835,7 +5829,7 @@
       <c r="I33" s="12"/>
       <c r="J33" s="18"/>
     </row>
-    <row r="34" ht="115.2" spans="1:10">
+    <row r="34" ht="123" spans="1:10">
       <c r="A34" s="10"/>
       <c r="B34" s="16" t="s">
         <v>84</v>
@@ -5861,7 +5855,7 @@
       <c r="I34" s="12"/>
       <c r="J34" s="18"/>
     </row>
-    <row r="35" ht="115.2" spans="1:10">
+    <row r="35" ht="123" spans="1:10">
       <c r="A35" s="10"/>
       <c r="B35" s="16" t="s">
         <v>88</v>
@@ -5887,7 +5881,7 @@
       <c r="I35" s="12"/>
       <c r="J35" s="18"/>
     </row>
-    <row r="36" ht="115.2" spans="1:10">
+    <row r="36" ht="123" spans="1:10">
       <c r="A36" s="10"/>
       <c r="B36" s="16" t="s">
         <v>92</v>
@@ -5913,7 +5907,7 @@
       <c r="I36" s="12"/>
       <c r="J36" s="18"/>
     </row>
-    <row r="37" ht="115.2" spans="1:10">
+    <row r="37" ht="123" spans="1:10">
       <c r="A37" s="10"/>
       <c r="B37" s="16" t="s">
         <v>96</v>
@@ -5939,7 +5933,7 @@
       <c r="I37" s="12"/>
       <c r="J37" s="18"/>
     </row>
-    <row r="38" ht="115.2" spans="1:10">
+    <row r="38" ht="123" spans="1:10">
       <c r="A38" s="10"/>
       <c r="B38" s="16" t="s">
         <v>100</v>
@@ -5965,7 +5959,7 @@
       <c r="I38" s="12"/>
       <c r="J38" s="18"/>
     </row>
-    <row r="39" ht="129.6" spans="1:10">
+    <row r="39" ht="123" spans="1:10">
       <c r="A39" s="10"/>
       <c r="B39" s="16" t="s">
         <v>104</v>
@@ -5991,7 +5985,7 @@
       <c r="I39" s="12"/>
       <c r="J39" s="18"/>
     </row>
-    <row r="40" ht="115.2" spans="1:10">
+    <row r="40" ht="123" spans="1:10">
       <c r="A40" s="10"/>
       <c r="B40" s="16" t="s">
         <v>108</v>
@@ -6017,7 +6011,7 @@
       <c r="I40" s="12"/>
       <c r="J40" s="18"/>
     </row>
-    <row r="41" ht="115.2" spans="1:10">
+    <row r="41" ht="123" spans="1:10">
       <c r="A41" s="10"/>
       <c r="B41" s="16" t="s">
         <v>112</v>
@@ -6043,7 +6037,7 @@
       <c r="I41" s="12"/>
       <c r="J41" s="18"/>
     </row>
-    <row r="42" ht="115.2" spans="1:10">
+    <row r="42" ht="123" spans="1:10">
       <c r="A42" s="10"/>
       <c r="B42" s="16" t="s">
         <v>116</v>
@@ -6069,7 +6063,7 @@
       <c r="I42" s="12"/>
       <c r="J42" s="18"/>
     </row>
-    <row r="43" ht="115.2" spans="1:10">
+    <row r="43" ht="123" spans="1:10">
       <c r="A43" s="10"/>
       <c r="B43" s="16" t="s">
         <v>121</v>
@@ -6095,7 +6089,7 @@
       <c r="I43" s="12"/>
       <c r="J43" s="18"/>
     </row>
-    <row r="44" ht="115.2" spans="1:10">
+    <row r="44" ht="123" spans="1:10">
       <c r="A44" s="10"/>
       <c r="B44" s="16" t="s">
         <v>125</v>
@@ -6121,7 +6115,7 @@
       <c r="I44" s="12"/>
       <c r="J44" s="18"/>
     </row>
-    <row r="45" ht="115.2" spans="1:10">
+    <row r="45" ht="123" spans="1:10">
       <c r="A45" s="10"/>
       <c r="B45" s="16" t="s">
         <v>129</v>
@@ -6147,7 +6141,7 @@
       <c r="I45" s="12"/>
       <c r="J45" s="18"/>
     </row>
-    <row r="46" ht="115.2" spans="1:10">
+    <row r="46" ht="123" spans="1:10">
       <c r="A46" s="10"/>
       <c r="B46" s="16" t="s">
         <v>133</v>
@@ -6173,7 +6167,7 @@
       <c r="I46" s="12"/>
       <c r="J46" s="18"/>
     </row>
-    <row r="47" ht="115.2" spans="1:10">
+    <row r="47" ht="123" spans="1:10">
       <c r="A47" s="10"/>
       <c r="B47" s="16" t="s">
         <v>137</v>
@@ -6199,7 +6193,7 @@
       <c r="I47" s="12"/>
       <c r="J47" s="18"/>
     </row>
-    <row r="48" ht="115.2" spans="1:10">
+    <row r="48" ht="123" spans="1:10">
       <c r="A48" s="10"/>
       <c r="B48" s="16" t="s">
         <v>141</v>
@@ -6225,7 +6219,7 @@
       <c r="I48" s="12"/>
       <c r="J48" s="18"/>
     </row>
-    <row r="49" ht="115.2" spans="1:10">
+    <row r="49" ht="123" spans="1:10">
       <c r="A49" s="10"/>
       <c r="B49" s="16" t="s">
         <v>145</v>
@@ -6251,7 +6245,7 @@
       <c r="I49" s="12"/>
       <c r="J49" s="18"/>
     </row>
-    <row r="50" ht="115.2" spans="1:10">
+    <row r="50" ht="123" spans="1:10">
       <c r="A50" s="10"/>
       <c r="B50" s="16" t="s">
         <v>150</v>
@@ -6277,7 +6271,7 @@
       <c r="I50" s="12"/>
       <c r="J50" s="18"/>
     </row>
-    <row r="51" ht="115.2" spans="1:10">
+    <row r="51" ht="123" spans="1:10">
       <c r="A51" s="10"/>
       <c r="B51" s="16" t="s">
         <v>154</v>
@@ -6303,7 +6297,7 @@
       <c r="I51" s="12"/>
       <c r="J51" s="18"/>
     </row>
-    <row r="52" ht="115.2" spans="1:10">
+    <row r="52" ht="123" spans="1:10">
       <c r="A52" s="10"/>
       <c r="B52" s="16" t="s">
         <v>158</v>
@@ -6329,7 +6323,7 @@
       <c r="I52" s="12"/>
       <c r="J52" s="18"/>
     </row>
-    <row r="53" ht="115.2" spans="1:10">
+    <row r="53" ht="123" spans="1:10">
       <c r="A53" s="10"/>
       <c r="B53" s="16" t="s">
         <v>163</v>
@@ -6355,7 +6349,7 @@
       <c r="I53" s="12"/>
       <c r="J53" s="18"/>
     </row>
-    <row r="54" ht="115.2" spans="1:10">
+    <row r="54" ht="123" spans="1:10">
       <c r="A54" s="10"/>
       <c r="B54" s="16" t="s">
         <v>167</v>
@@ -6381,7 +6375,7 @@
       <c r="I54" s="12"/>
       <c r="J54" s="18"/>
     </row>
-    <row r="55" ht="129.6" spans="1:10">
+    <row r="55" ht="138.6" spans="1:10">
       <c r="A55" s="10"/>
       <c r="B55" s="16" t="s">
         <v>170</v>
@@ -6407,7 +6401,7 @@
       <c r="I55" s="12"/>
       <c r="J55" s="18"/>
     </row>
-    <row r="56" ht="115.2" spans="1:10">
+    <row r="56" ht="123" spans="1:10">
       <c r="A56" s="10"/>
       <c r="B56" s="16" t="s">
         <v>174</v>
@@ -6433,7 +6427,7 @@
       <c r="I56" s="12"/>
       <c r="J56" s="18"/>
     </row>
-    <row r="57" ht="115.2" spans="1:10">
+    <row r="57" ht="123" spans="1:10">
       <c r="A57" s="10"/>
       <c r="B57" s="16" t="s">
         <v>178</v>
@@ -6459,7 +6453,7 @@
       <c r="I57" s="12"/>
       <c r="J57" s="18"/>
     </row>
-    <row r="58" ht="115.2" spans="1:10">
+    <row r="58" ht="123" spans="1:10">
       <c r="A58" s="10"/>
       <c r="B58" s="16" t="s">
         <v>182</v>
@@ -6485,7 +6479,7 @@
       <c r="I58" s="12"/>
       <c r="J58" s="18"/>
     </row>
-    <row r="59" ht="115.2" spans="1:10">
+    <row r="59" ht="123" spans="1:10">
       <c r="A59" s="10"/>
       <c r="B59" s="16" t="s">
         <v>186</v>
@@ -6511,7 +6505,7 @@
       <c r="I59" s="12"/>
       <c r="J59" s="18"/>
     </row>
-    <row r="60" ht="115.2" spans="1:10">
+    <row r="60" ht="123" spans="1:10">
       <c r="A60" s="10"/>
       <c r="B60" s="16" t="s">
         <v>190</v>
@@ -6537,7 +6531,7 @@
       <c r="I60" s="12"/>
       <c r="J60" s="18"/>
     </row>
-    <row r="61" ht="115.2" spans="1:10">
+    <row r="61" ht="123" spans="1:10">
       <c r="A61" s="10"/>
       <c r="B61" s="16" t="s">
         <v>195</v>
@@ -6563,7 +6557,7 @@
       <c r="I61" s="12"/>
       <c r="J61" s="18"/>
     </row>
-    <row r="62" ht="115.2" spans="1:10">
+    <row r="62" ht="123" spans="1:10">
       <c r="A62" s="10"/>
       <c r="B62" s="16" t="s">
         <v>199</v>
@@ -6589,7 +6583,7 @@
       <c r="I62" s="12"/>
       <c r="J62" s="18"/>
     </row>
-    <row r="63" ht="115.2" spans="1:10">
+    <row r="63" ht="123" spans="1:10">
       <c r="A63" s="10"/>
       <c r="B63" s="16" t="s">
         <v>203</v>
@@ -6615,7 +6609,7 @@
       <c r="I63" s="12"/>
       <c r="J63" s="18"/>
     </row>
-    <row r="64" ht="115.2" spans="1:10">
+    <row r="64" ht="123" spans="1:10">
       <c r="A64" s="10"/>
       <c r="B64" s="16" t="s">
         <v>207</v>
@@ -6641,7 +6635,7 @@
       <c r="I64" s="12"/>
       <c r="J64" s="18"/>
     </row>
-    <row r="65" ht="115.2" spans="1:10">
+    <row r="65" ht="123" spans="1:10">
       <c r="A65" s="10"/>
       <c r="B65" s="16" t="s">
         <v>211</v>
@@ -6667,7 +6661,7 @@
       <c r="I65" s="12"/>
       <c r="J65" s="18"/>
     </row>
-    <row r="66" ht="115.2" spans="1:10">
+    <row r="66" ht="123" spans="1:10">
       <c r="A66" s="10"/>
       <c r="B66" s="16" t="s">
         <v>214</v>
@@ -6693,7 +6687,7 @@
       <c r="I66" s="12"/>
       <c r="J66" s="18"/>
     </row>
-    <row r="67" ht="115.2" spans="1:10">
+    <row r="67" ht="123" spans="1:10">
       <c r="A67" s="10"/>
       <c r="B67" s="16" t="s">
         <v>219</v>
@@ -6719,7 +6713,7 @@
       <c r="I67" s="12"/>
       <c r="J67" s="18"/>
     </row>
-    <row r="68" ht="115.2" spans="1:10">
+    <row r="68" ht="123" spans="1:10">
       <c r="A68" s="10"/>
       <c r="B68" s="16" t="s">
         <v>223</v>
@@ -6745,7 +6739,7 @@
       <c r="I68" s="12"/>
       <c r="J68" s="18"/>
     </row>
-    <row r="69" ht="115.2" spans="1:10">
+    <row r="69" ht="123" spans="1:10">
       <c r="A69" s="10"/>
       <c r="B69" s="16" t="s">
         <v>229</v>
@@ -6771,7 +6765,7 @@
       <c r="I69" s="12"/>
       <c r="J69" s="18"/>
     </row>
-    <row r="70" ht="115.2" spans="1:10">
+    <row r="70" ht="123" spans="1:10">
       <c r="A70" s="10"/>
       <c r="B70" s="16" t="s">
         <v>234</v>
@@ -6797,7 +6791,7 @@
       <c r="I70" s="12"/>
       <c r="J70" s="18"/>
     </row>
-    <row r="71" s="2" customFormat="1" ht="115.2" spans="1:10">
+    <row r="71" s="2" customFormat="1" ht="123" spans="1:10">
       <c r="A71" s="22"/>
       <c r="B71" s="23" t="s">
         <v>240</v>
@@ -6820,10 +6814,10 @@
       <c r="H71" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="I71" s="29"/>
-      <c r="J71" s="30"/>
-    </row>
-    <row r="72" s="2" customFormat="1" ht="115.2" spans="1:10">
+      <c r="I71" s="27"/>
+      <c r="J71" s="28"/>
+    </row>
+    <row r="72" s="2" customFormat="1" ht="123" spans="1:10">
       <c r="A72" s="22"/>
       <c r="B72" s="16" t="s">
         <v>245</v>
@@ -6846,10 +6840,10 @@
       <c r="H72" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="I72" s="29"/>
-      <c r="J72" s="30"/>
-    </row>
-    <row r="73" s="2" customFormat="1" ht="115.2" spans="1:10">
+      <c r="I72" s="27"/>
+      <c r="J72" s="28"/>
+    </row>
+    <row r="73" s="2" customFormat="1" ht="123" spans="1:10">
       <c r="A73" s="22"/>
       <c r="B73" s="23" t="s">
         <v>250</v>
@@ -6872,10 +6866,10 @@
       <c r="H73" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="I73" s="29"/>
-      <c r="J73" s="30"/>
-    </row>
-    <row r="74" s="2" customFormat="1" ht="115.2" spans="1:10">
+      <c r="I73" s="27"/>
+      <c r="J73" s="28"/>
+    </row>
+    <row r="74" s="2" customFormat="1" ht="123" spans="1:10">
       <c r="A74" s="22"/>
       <c r="B74" s="16" t="s">
         <v>255</v>
@@ -6898,10 +6892,10 @@
       <c r="H74" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="I74" s="29"/>
-      <c r="J74" s="30"/>
-    </row>
-    <row r="75" s="2" customFormat="1" ht="115.2" spans="1:10">
+      <c r="I74" s="27"/>
+      <c r="J74" s="28"/>
+    </row>
+    <row r="75" s="2" customFormat="1" ht="123" spans="1:10">
       <c r="A75" s="22"/>
       <c r="B75" s="23" t="s">
         <v>260</v>
@@ -6924,10 +6918,10 @@
       <c r="H75" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="I75" s="29"/>
-      <c r="J75" s="30"/>
-    </row>
-    <row r="76" s="2" customFormat="1" ht="115.2" spans="1:10">
+      <c r="I75" s="27"/>
+      <c r="J75" s="28"/>
+    </row>
+    <row r="76" s="2" customFormat="1" ht="123" spans="1:10">
       <c r="A76" s="22"/>
       <c r="B76" s="16" t="s">
         <v>265</v>
@@ -6950,10 +6944,10 @@
       <c r="H76" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="I76" s="29"/>
-      <c r="J76" s="30"/>
-    </row>
-    <row r="77" s="1" customFormat="1" ht="115.2" spans="1:10">
+      <c r="I76" s="27"/>
+      <c r="J76" s="28"/>
+    </row>
+    <row r="77" s="1" customFormat="1" ht="123" spans="1:10">
       <c r="A77" s="13"/>
       <c r="B77" s="14" t="s">
         <v>270</v>
@@ -6979,7 +6973,7 @@
       <c r="I77" s="20"/>
       <c r="J77" s="21"/>
     </row>
-    <row r="78" customFormat="1" ht="115.2" spans="1:10">
+    <row r="78" customFormat="1" ht="123" spans="1:10">
       <c r="A78" s="10"/>
       <c r="B78" s="16" t="s">
         <v>277</v>
@@ -7005,7 +6999,7 @@
       <c r="I78" s="12"/>
       <c r="J78" s="18"/>
     </row>
-    <row r="79" ht="115.2" spans="1:10">
+    <row r="79" ht="123" spans="1:10">
       <c r="A79" s="10"/>
       <c r="B79" s="23" t="s">
         <v>281</v>
@@ -7031,7 +7025,7 @@
       <c r="I79" s="12"/>
       <c r="J79" s="18"/>
     </row>
-    <row r="80" s="2" customFormat="1" ht="115.2" spans="1:10">
+    <row r="80" s="2" customFormat="1" ht="123" spans="1:10">
       <c r="A80" s="22"/>
       <c r="B80" s="16" t="s">
         <v>286</v>
@@ -7054,10 +7048,10 @@
       <c r="H80" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="I80" s="29"/>
-      <c r="J80" s="30"/>
-    </row>
-    <row r="81" ht="115.2" spans="1:10">
+      <c r="I80" s="27"/>
+      <c r="J80" s="28"/>
+    </row>
+    <row r="81" ht="123" spans="1:10">
       <c r="A81" s="10"/>
       <c r="B81" s="23" t="s">
         <v>290</v>
@@ -7083,7 +7077,7 @@
       <c r="I81" s="12"/>
       <c r="J81" s="18"/>
     </row>
-    <row r="82" ht="115.2" spans="1:10">
+    <row r="82" ht="123" spans="1:10">
       <c r="A82" s="10"/>
       <c r="B82" s="16" t="s">
         <v>294</v>
@@ -7109,7 +7103,7 @@
       <c r="I82" s="12"/>
       <c r="J82" s="18"/>
     </row>
-    <row r="83" ht="115.2" spans="1:9">
+    <row r="83" ht="123" spans="1:9">
       <c r="A83" s="10"/>
       <c r="B83" s="23" t="s">
         <v>298</v>
@@ -7150,129 +7144,129 @@
       <c r="K85" s="5"/>
     </row>
     <row r="86" spans="1:11">
-      <c r="A86" s="26" t="s">
+      <c r="A86" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B86" s="27" t="s">
+      <c r="B86" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C86" s="27"/>
-      <c r="D86" s="27"/>
-      <c r="E86" s="27"/>
-      <c r="F86" s="27"/>
-      <c r="G86" s="27"/>
-      <c r="H86" s="27"/>
-      <c r="I86" s="27"/>
-      <c r="J86" s="27"/>
-      <c r="K86" s="27"/>
+      <c r="C86" s="26"/>
+      <c r="D86" s="26"/>
+      <c r="E86" s="26"/>
+      <c r="F86" s="26"/>
+      <c r="G86" s="26"/>
+      <c r="H86" s="26"/>
+      <c r="I86" s="26"/>
+      <c r="J86" s="26"/>
+      <c r="K86" s="26"/>
     </row>
     <row r="87" spans="1:11">
-      <c r="A87" s="26" t="s">
+      <c r="A87" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B87" s="27" t="s">
+      <c r="B87" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C87" s="27"/>
-      <c r="D87" s="27"/>
-      <c r="E87" s="27"/>
-      <c r="F87" s="27"/>
-      <c r="G87" s="27"/>
-      <c r="H87" s="27"/>
-      <c r="I87" s="27"/>
-      <c r="J87" s="27"/>
-      <c r="K87" s="26"/>
+      <c r="C87" s="26"/>
+      <c r="D87" s="26"/>
+      <c r="E87" s="26"/>
+      <c r="F87" s="26"/>
+      <c r="G87" s="26"/>
+      <c r="H87" s="26"/>
+      <c r="I87" s="26"/>
+      <c r="J87" s="26"/>
+      <c r="K87" s="10"/>
     </row>
     <row r="88" spans="1:11">
-      <c r="A88" s="26" t="s">
+      <c r="A88" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B88" s="26" t="s">
+      <c r="B88" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="C88" s="26" t="s">
+      <c r="C88" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="D88" s="26" t="s">
+      <c r="D88" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E88" s="26" t="s">
+      <c r="E88" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="F88" s="26" t="s">
+      <c r="F88" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="G88" s="26" t="s">
+      <c r="G88" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H88" s="26" t="s">
+      <c r="H88" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="I88" s="26" t="s">
+      <c r="I88" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J88" s="26" t="s">
+      <c r="J88" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="K88" s="26"/>
-    </row>
-    <row r="89" ht="57.6" spans="1:11">
-      <c r="A89" s="26"/>
-      <c r="B89" s="26" t="s">
+      <c r="K88" s="10"/>
+    </row>
+    <row r="89" ht="60.6" spans="1:11">
+      <c r="A89" s="10"/>
+      <c r="B89" s="10" t="s">
         <v>308</v>
       </c>
-      <c r="C89" s="28" t="s">
+      <c r="C89" s="17" t="s">
         <v>309</v>
       </c>
-      <c r="D89" s="26" t="s">
+      <c r="D89" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E89" s="28" t="s">
+      <c r="E89" s="17" t="s">
         <v>310</v>
       </c>
-      <c r="F89" s="26">
+      <c r="F89" s="10">
         <v>2</v>
       </c>
-      <c r="G89" s="28" t="s">
+      <c r="G89" s="17" t="s">
         <v>311</v>
       </c>
-      <c r="H89" s="28" t="s">
+      <c r="H89" s="17" t="s">
         <v>312</v>
       </c>
-      <c r="I89" s="28" t="s">
+      <c r="I89" s="17" t="s">
         <v>313</v>
       </c>
-      <c r="J89" s="26"/>
-      <c r="K89" s="26"/>
-    </row>
-    <row r="90" ht="86.4" spans="1:11">
-      <c r="A90" s="26"/>
-      <c r="B90" s="26" t="s">
+      <c r="J89" s="10"/>
+      <c r="K89" s="10"/>
+    </row>
+    <row r="90" ht="78" spans="1:11">
+      <c r="A90" s="10"/>
+      <c r="B90" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="C90" s="28" t="s">
+      <c r="C90" s="17" t="s">
         <v>315</v>
       </c>
-      <c r="D90" s="26" t="s">
+      <c r="D90" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="E90" s="28" t="s">
+      <c r="E90" s="17" t="s">
         <v>315</v>
       </c>
-      <c r="F90" s="26">
+      <c r="F90" s="10">
         <v>2</v>
       </c>
-      <c r="G90" s="28" t="s">
+      <c r="G90" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="H90" s="28" t="s">
+      <c r="H90" s="17" t="s">
         <v>316</v>
       </c>
-      <c r="I90" s="26" t="s">
+      <c r="I90" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="J90" s="26"/>
-      <c r="K90" s="26"/>
+      <c r="J90" s="10"/>
+      <c r="K90" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -7301,7 +7295,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -7318,7 +7312,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>